<commit_message>
Removing comment anonymity - closes #2
</commit_message>
<xml_diff>
--- a/resources/Answer Template.xlsx
+++ b/resources/Answer Template.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="920" windowWidth="25120" windowHeight="15140" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="920" windowWidth="25120" windowHeight="15140" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>ATTENTION!</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>The Survey Tool uses this spreadsheet to contain answers, but DO NOT access this spreadsheet directly!</t>
+  </si>
+  <si>
+    <t>User</t>
   </si>
 </sst>
 </file>
@@ -519,7 +522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -725,16 +728,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:20" ht="12.75" customHeight="1">
+    <row r="1" spans="1:21" ht="12.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -742,21 +745,23 @@
         <v>30</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -769,6 +774,7 @@
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>